<commit_message>
Added Review Time to Excel document
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/327F19256DF589A6/Documente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VVSS\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EC7CD94-1E23-4075-BBE5-C359E871BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F4B3D8-E3E2-46B0-AEF5-92AFFC88F0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="13680" tabRatio="650" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -426,7 +426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,8 +623,19 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,7 +658,16 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,26 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,23 +991,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="5" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="8.86328125" style="5"/>
+    <col min="2" max="2" width="12.265625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="16.265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.3984375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="5"/>
     <col min="9" max="9" width="21" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="10" max="10" width="14.3984375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1017,31 +1017,31 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1049,93 +1049,93 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -1155,9 +1155,9 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="45.75">
+    <row r="10" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="16"/>
-      <c r="B10" s="35">
+      <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1175,9 +1175,9 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="106.5">
+    <row r="11" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A11" s="16"/>
-      <c r="B11" s="35">
+      <c r="B11" s="19">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1196,9 +1196,9 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="45.75">
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="16"/>
-      <c r="B12" s="35">
+      <c r="B12" s="19">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1215,9 +1215,9 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="45.75">
+    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
-      <c r="B13" s="35">
+      <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1234,9 +1234,9 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="45.75">
+    <row r="14" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
-      <c r="B14" s="35">
+      <c r="B14" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1253,9 +1253,9 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" ht="45.75">
+    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
-      <c r="B15" s="35">
+      <c r="B15" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1274,9 +1274,9 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" ht="45.75">
+    <row r="16" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
-      <c r="B16" s="35">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1293,8 +1293,8 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1302,85 +1302,87 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="35">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="35">
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="35">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B21" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="35">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="35">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="35">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="35">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B27" s="16"/>
       <c r="C27" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1403,22 +1405,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="5" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="5"/>
-    <col min="9" max="9" width="22.140625" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="8.86328125" style="5"/>
+    <col min="2" max="2" width="12.265625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="16.265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.3984375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="5"/>
+    <col min="9" max="9" width="22.1328125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1428,31 +1430,31 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1460,93 +1462,93 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -1566,9 +1568,9 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="45.75">
+    <row r="10" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="16"/>
-      <c r="B10" s="35">
+      <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1584,9 +1586,9 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="45.75">
+    <row r="11" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="16"/>
-      <c r="B11" s="35">
+      <c r="B11" s="19">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1605,9 +1607,9 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="45.75">
+    <row r="12" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="16"/>
-      <c r="B12" s="35">
+      <c r="B12" s="19">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1626,9 +1628,9 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="30.75">
+    <row r="13" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
-      <c r="B13" s="35">
+      <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1645,9 +1647,9 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="30.75">
+    <row r="14" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
-      <c r="B14" s="35">
+      <c r="B14" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1664,9 +1666,9 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" ht="60.75">
+    <row r="15" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
-      <c r="B15" s="35">
+      <c r="B15" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1685,9 +1687,9 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
-      <c r="B16" s="35">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1700,8 +1702,8 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1709,8 +1711,8 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1718,8 +1720,8 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1727,8 +1729,8 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1736,8 +1738,8 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B21" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1745,8 +1747,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1754,8 +1756,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1763,8 +1765,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1772,8 +1774,8 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1781,8 +1783,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B26" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1790,13 +1792,15 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" s="16"/>
       <c r="C28" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="11"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1819,23 +1823,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="5"/>
+    <col min="2" max="2" width="12.265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" style="5" customWidth="1"/>
     <col min="4" max="4" width="18" style="5" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="5" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="5"/>
-    <col min="9" max="9" width="26.7109375" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="5"/>
+    <col min="5" max="5" width="41.3984375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="5"/>
+    <col min="9" max="9" width="26.73046875" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1845,31 +1849,31 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1877,61 +1881,61 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.45" customHeight="1">
+    <row r="6" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -1947,23 +1951,23 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -1983,9 +1987,9 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="45.75">
+    <row r="10" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="16"/>
-      <c r="B10" s="35">
+      <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2003,16 +2007,16 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="45.75">
+    <row r="11" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="16"/>
-      <c r="B11" s="35">
+      <c r="B11" s="19">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="17" t="s">
         <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2024,9 +2028,9 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="76.5">
+    <row r="12" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A12" s="16"/>
-      <c r="B12" s="35">
+      <c r="B12" s="19">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -2045,9 +2049,9 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="137.25">
+    <row r="13" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
-      <c r="B13" s="35">
+      <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2066,9 +2070,9 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="45.75">
+    <row r="14" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
-      <c r="B14" s="35">
+      <c r="B14" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2085,9 +2089,9 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" ht="30.75">
+    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
-      <c r="B15" s="35">
+      <c r="B15" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2106,9 +2110,9 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
-      <c r="B16" s="35">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2121,8 +2125,8 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2130,8 +2134,8 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2139,8 +2143,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2148,8 +2152,8 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2157,8 +2161,8 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B21" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2166,8 +2170,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2175,8 +2179,8 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2184,8 +2188,8 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B24" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2193,8 +2197,8 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2202,8 +2206,8 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B26" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -2211,8 +2215,8 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B27" s="19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2220,8 +2224,8 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B28" s="19">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2229,8 +2233,8 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B29" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2238,8 +2242,8 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B30" s="19">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2247,13 +2251,15 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B32" s="16"/>
       <c r="C32" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2276,24 +2282,24 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="5"/>
+    <col min="2" max="2" width="12.265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" style="5" customWidth="1"/>
     <col min="4" max="4" width="18" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="5" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="5"/>
-    <col min="9" max="9" width="26.7109375" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="5"/>
+    <col min="5" max="5" width="23.86328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="5" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" style="5"/>
+    <col min="9" max="9" width="26.73046875" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2303,31 +2309,31 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -2335,75 +2341,75 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="19">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -2425,9 +2431,9 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="76.5">
+    <row r="10" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A10" s="16"/>
-      <c r="B10" s="35">
+      <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -2447,9 +2453,9 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="121.5">
+    <row r="11" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A11" s="16"/>
-      <c r="B11" s="35">
+      <c r="B11" s="19">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -2470,9 +2476,9 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="121.5">
+    <row r="12" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A12" s="16"/>
-      <c r="B12" s="35">
+      <c r="B12" s="19">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -2493,9 +2499,9 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="409.6">
+    <row r="13" spans="1:10" ht="399" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
-      <c r="B13" s="35">
+      <c r="B13" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2516,9 +2522,9 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="60.75">
+    <row r="14" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
-      <c r="B14" s="35">
+      <c r="B14" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2537,16 +2543,16 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" ht="152.25">
+    <row r="15" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
-      <c r="B15" s="35">
+      <c r="B15" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="18" t="s">
         <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -2560,9 +2566,9 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" ht="244.5">
+    <row r="16" spans="1:10" ht="213.75" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
-      <c r="B16" s="35">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2583,8 +2589,8 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2593,8 +2599,8 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2603,8 +2609,8 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B19" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2613,8 +2619,8 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2623,8 +2629,8 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B21" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2633,8 +2639,8 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B22" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2643,8 +2649,8 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B23" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2653,8 +2659,8 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B24" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2663,8 +2669,8 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B25" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2673,8 +2679,8 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B26" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -2683,8 +2689,8 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B27" s="19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2693,8 +2699,8 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B28" s="19">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2703,8 +2709,8 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B29" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2713,8 +2719,8 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B30" s="19">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2723,16 +2729,16 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32" s="16"/>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="15"/>
     </row>
-    <row r="35" spans="6:6">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F35" s="16"/>
     </row>
   </sheetData>

</xml_diff>